<commit_message>
modal dialog art/implement, level 1 flow
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D9A299-9086-4350-9F0F-463E9F71B81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8541C98-D35F-4B4E-B8C4-AAD1D9839CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="3270" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Key</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>Project Triumph</t>
+  </si>
+  <si>
+    <t>Testing, testing, 1…2…3…</t>
+  </si>
+  <si>
+    <t>test_0</t>
   </si>
 </sst>
 </file>
@@ -390,7 +396,7 @@
   <dimension ref="A1:D198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +430,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>

</xml_diff>

<commit_message>
options ui, wtf was I thinking with level 3, refactoring
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8541C98-D35F-4B4E-B8C4-AAD1D9839CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A69A8F-B4F7-4A5F-913E-2D3F13267610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="3270" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3885" yWindow="6645" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Key</t>
   </si>
@@ -44,6 +44,60 @@
   </si>
   <si>
     <t>test_0</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>SPEECH</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
+  </si>
+  <si>
+    <t>newGame</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
   </si>
 </sst>
 </file>
@@ -396,7 +450,7 @@
   <dimension ref="A1:D198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,31 +492,76 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>

</xml_diff>

<commit_message>
rearrange stuff, title screen, better victory flow
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A69A8F-B4F7-4A5F-913E-2D3F13267610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9258840-805E-4D0B-A0AD-2B890D64CC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3885" yWindow="6645" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="6750" windowWidth="26865" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Key</t>
   </si>
@@ -37,9 +37,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>Project Triumph</t>
-  </si>
-  <si>
     <t>Testing, testing, 1…2…3…</t>
   </si>
   <si>
@@ -98,6 +95,21 @@
   </si>
   <si>
     <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>RENEGADEWARE</t>
+  </si>
+  <si>
+    <t>credits_music</t>
+  </si>
+  <si>
+    <t>Music and Sound by Winfield B. Carson V\n\nSinger Katya Hall</t>
+  </si>
+  <si>
+    <t>Mighty Aries\n&lt;size=36&gt;and the&lt;/size&gt;\nMovement of Energy</t>
   </si>
 </sst>
 </file>
@@ -447,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D198"/>
+  <dimension ref="A1:D200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,109 +492,119 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -816,55 +838,55 @@
       <c r="B96" s="2"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="5"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="3"/>
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="2"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="5"/>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="3"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="3"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="3"/>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="3"/>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="3"/>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="3"/>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="3"/>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="3"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" s="3"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111" s="3"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" s="3"/>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" s="3"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" s="3"/>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="4"/>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="5"/>
+      <c r="B153" s="3"/>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="4"/>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="4"/>
+      <c r="B156" s="5"/>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="4"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="5"/>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" s="5"/>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158" s="4"/>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159" s="4"/>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162" s="4"/>
+      <c r="B162" s="5"/>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="5"/>
@@ -873,7 +895,7 @@
       <c r="B164" s="4"/>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B165" s="4"/>
+      <c r="B165" s="5"/>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="4"/>
@@ -885,31 +907,31 @@
       <c r="B168" s="4"/>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169" s="5"/>
+      <c r="B169" s="4"/>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B170" s="3"/>
+      <c r="B170" s="4"/>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171" s="4"/>
-    </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B174" s="3"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="4"/>
-    </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="3"/>
+      <c r="B171" s="5"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B172" s="3"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B173" s="4"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B176" s="3"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B179" s="4"/>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180" s="5"/>
-    </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" s="4"/>
+      <c r="B180" s="3"/>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="4"/>
+      <c r="B182" s="5"/>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="4"/>
@@ -921,31 +943,37 @@
       <c r="B185" s="4"/>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B186" s="5"/>
-    </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B189" s="3"/>
-    </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B190" s="3"/>
+      <c r="B186" s="4"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B187" s="4"/>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B188" s="5"/>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" s="3"/>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B192" s="5"/>
+      <c r="B192" s="3"/>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B193" s="4"/>
+      <c r="B193" s="3"/>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="5"/>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B197" s="3"/>
-    </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B198" s="3"/>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B195" s="4"/>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B196" s="5"/>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B199" s="3"/>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B200" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed some physics issue, tweaked level 3 and level 5, pause on options
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E691FDF0-4D46-47A8-A1EC-2E3742C5B43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACECD8E-F0DC-4A36-ACB0-EC9EAC45F544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18645" yWindow="5505" windowWidth="17910" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14775" yWindow="5640" windowWidth="17910" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -571,18 +571,9 @@
     <t>Nicely done! As you can see, the energy of motion moved from one object to another.</t>
   </si>
   <si>
-    <t>The energy released from the spring plunger has caused a series of movement, from one rock all the way to that other rock.</t>
-  </si>
-  <si>
     <t>Now let’s see if you can ring these other bells!</t>
   </si>
   <si>
-    <t>You’ll need to adjust the direction of this rock so it can hit the second platform.</t>
-  </si>
-  <si>
-    <t>You’ll also need to adjust the position of this rock so it can launch, and hit both bells.</t>
-  </si>
-  <si>
     <t>Here we have a spirit that provides us an everlasting flow of water.</t>
   </si>
   <si>
@@ -632,6 +623,15 @@
   </si>
   <si>
     <t>Also remember to keep the fire well fed with coal and oxygen!</t>
+  </si>
+  <si>
+    <t>Let me adjust this so that it can hit the second platform!</t>
+  </si>
+  <si>
+    <t>You’re going to need to adjust the position of this rock in order to hit both bells.</t>
+  </si>
+  <si>
+    <t>The energy released from the spring plunger has caused a series of movement, from one rock to another.</t>
   </si>
 </sst>
 </file>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,8 +1442,8 @@
       <c r="A57" t="s">
         <v>86</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>183</v>
+      <c r="B57" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1451,23 +1451,23 @@
         <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>88</v>
       </c>
-      <c r="B59" t="s">
-        <v>185</v>
+      <c r="B59" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>89</v>
       </c>
-      <c r="B60" t="s">
-        <v>186</v>
+      <c r="B60" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1491,7 +1491,7 @@
         <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>98</v>
       </c>
       <c r="B64" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1571,7 +1571,7 @@
         <v>113</v>
       </c>
       <c r="B73" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
         <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1603,7 +1603,7 @@
         <v>119</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>128</v>
       </c>
       <c r="B78" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
         <v>129</v>
       </c>
       <c r="B79" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
         <v>123</v>
       </c>
       <c r="B80" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1643,7 +1643,7 @@
         <v>125</v>
       </c>
       <c r="B82" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1651,7 +1651,7 @@
         <v>126</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
         <v>132</v>
       </c>
       <c r="B86" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>143</v>
       </c>
       <c r="B92" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1731,7 +1731,7 @@
         <v>144</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1739,7 +1739,7 @@
         <v>145</v>
       </c>
       <c r="B94" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1747,7 +1747,7 @@
         <v>146</v>
       </c>
       <c r="B95" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1755,7 +1755,7 @@
         <v>147</v>
       </c>
       <c r="B96" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1763,7 +1763,7 @@
         <v>148</v>
       </c>
       <c r="B97" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
disable options during loading, added keyboard skipping for dialog, change wait transition mode for modals
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACECD8E-F0DC-4A36-ACB0-EC9EAC45F544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B984A972-BBBF-4E37-920A-2A9104E8ECF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14775" yWindow="5640" windowWidth="17910" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,9 +550,6 @@
     <t>Due to the light, the bell is able to vibrate causing it to make another type of energy: sound.</t>
   </si>
   <si>
-    <t>As you can see, we are able to change from one energy into another. From light to sound energy.</t>
-  </si>
-  <si>
     <t>But of course, none of this is possible without your actions. Your own energy is what brings these to life!</t>
   </si>
   <si>
@@ -595,9 +592,6 @@
     <t>Well, that’s what these coals are for. Coals provide fire with the energy to release heat.</t>
   </si>
   <si>
-    <t>Whew! That’s a lot of energy movement from one thing to another!</t>
-  </si>
-  <si>
     <t>Well, electrical energy is really easy to move at a long distance. Think of the electrical poles around your home.</t>
   </si>
   <si>
@@ -632,6 +626,12 @@
   </si>
   <si>
     <t>The energy released from the spring plunger has caused a series of movement, from one rock to another.</t>
+  </si>
+  <si>
+    <t>As you can see, we are able to change from one energy into another. It changes from light to sound energy.</t>
+  </si>
+  <si>
+    <t>Phew! That’s a lot of energy movement from one thing to another!</t>
   </si>
 </sst>
 </file>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,7 +1347,7 @@
         <v>71</v>
       </c>
       <c r="B45" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1355,7 +1355,7 @@
         <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1363,7 +1363,7 @@
         <v>73</v>
       </c>
       <c r="B47" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1371,7 +1371,7 @@
         <v>74</v>
       </c>
       <c r="B48" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1387,7 +1387,7 @@
         <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1395,7 +1395,7 @@
         <v>77</v>
       </c>
       <c r="B51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
         <v>85</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>86</v>
       </c>
       <c r="B57" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1451,7 +1451,7 @@
         <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1459,7 +1459,7 @@
         <v>88</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1467,7 +1467,7 @@
         <v>89</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1491,7 +1491,7 @@
         <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>98</v>
       </c>
       <c r="B64" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1571,7 +1571,7 @@
         <v>113</v>
       </c>
       <c r="B73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
         <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1603,7 +1603,7 @@
         <v>119</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>128</v>
       </c>
       <c r="B78" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
         <v>129</v>
       </c>
       <c r="B79" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
         <v>123</v>
       </c>
       <c r="B80" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1643,7 +1643,7 @@
         <v>125</v>
       </c>
       <c r="B82" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1651,7 +1651,7 @@
         <v>126</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
         <v>132</v>
       </c>
       <c r="B86" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>143</v>
       </c>
       <c r="B92" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1731,7 +1731,7 @@
         <v>144</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1739,7 +1739,7 @@
         <v>145</v>
       </c>
       <c r="B94" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1747,7 +1747,7 @@
         <v>146</v>
       </c>
       <c r="B95" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1755,7 +1755,7 @@
         <v>147</v>
       </c>
       <c r="B96" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1763,7 +1763,7 @@
         <v>148</v>
       </c>
       <c r="B97" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
a bunch of fixes and such
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B984A972-BBBF-4E37-920A-2A9104E8ECF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9981FF96-C25C-4245-81A9-E1ED7FFAA38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14775" yWindow="5640" windowWidth="17910" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="2940" windowWidth="20160" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>Key</t>
   </si>
@@ -115,18 +115,6 @@
     <t>intro_3</t>
   </si>
   <si>
-    <t>intro_4</t>
-  </si>
-  <si>
-    <t>intro_5</t>
-  </si>
-  <si>
-    <t>Welcome!</t>
-  </si>
-  <si>
-    <t>Energy provides us the power to act, and the ability to change. Though Aries is a bundle of energy, he is currently at rest.</t>
-  </si>
-  <si>
     <t>intro_0</t>
   </si>
   <si>
@@ -136,12 +124,6 @@
     <t>level_1_intro_1</t>
   </si>
   <si>
-    <t>level_1_intro_2</t>
-  </si>
-  <si>
-    <t>level_1_intro_3</t>
-  </si>
-  <si>
     <t>We will start with light.</t>
   </si>
   <si>
@@ -154,33 +136,18 @@
     <t>level_1_instruction_0</t>
   </si>
   <si>
-    <t>Simply move the contraption like so!</t>
-  </si>
-  <si>
     <t>level_1_outer_complete_0</t>
   </si>
   <si>
     <t>level_1_inner_complete_0</t>
   </si>
   <si>
-    <t>Great! Now just one more, and the light shall shine through!</t>
-  </si>
-  <si>
     <t>level_1_victory_1_0</t>
   </si>
   <si>
-    <t>As the warm light embraces Aries’s body, he begins to wake up!</t>
-  </si>
-  <si>
     <t>level_1_victory_2_0</t>
   </si>
   <si>
-    <t>level_1_victory_3_0</t>
-  </si>
-  <si>
-    <t>level_1_victory_3_1</t>
-  </si>
-  <si>
     <t>level_2_intro_0</t>
   </si>
   <si>
@@ -193,39 +160,15 @@
     <t>level_2_gem_instruct_0</t>
   </si>
   <si>
-    <t>level_2_gem_instruct_1</t>
-  </si>
-  <si>
-    <t>Go ahead and place the gem into the indicated slot.</t>
-  </si>
-  <si>
-    <t>Simply press the gem, and drag it into the slot as shown.</t>
-  </si>
-  <si>
     <t>level_2_gem_placed_0</t>
   </si>
   <si>
-    <t>Excellent! As you can see, the light energy is bouncing off of the gem towards a direction.</t>
-  </si>
-  <si>
     <t>level_2_gem_next_0</t>
   </si>
   <si>
-    <t>Now on to the next gem! Just like before, drag the object towards the indicated slot.</t>
-  </si>
-  <si>
     <t>level_2_gem_next_placed_0</t>
   </si>
   <si>
-    <t>We’re almost there. Now we just need to adjust the direction of the light towards the bell.</t>
-  </si>
-  <si>
-    <t>level_2_slot_instruct_0</t>
-  </si>
-  <si>
-    <t>All you need to do is press and drag the lever to rotate the slot.</t>
-  </si>
-  <si>
     <t>level_2_goal_1_reached_0</t>
   </si>
   <si>
@@ -238,15 +181,9 @@
     <t>level_2_goal_1_reached_2</t>
   </si>
   <si>
-    <t>level_2_goal_1_reached_3</t>
-  </si>
-  <si>
     <t>level_2_next_task_0</t>
   </si>
   <si>
-    <t>level_2_next_task_1</t>
-  </si>
-  <si>
     <t>level_3_intro_0</t>
   </si>
   <si>
@@ -286,9 +223,6 @@
     <t>level_3_goal_pointers_0</t>
   </si>
   <si>
-    <t>level_3_rotate_pointer_0</t>
-  </si>
-  <si>
     <t>level_3_slider_pointer_0</t>
   </si>
   <si>
@@ -304,9 +238,6 @@
     <t>Let’s go check out how this energy of motion works!</t>
   </si>
   <si>
-    <t>Excellent! Can you hear that? The bell is ringing joyously!</t>
-  </si>
-  <si>
     <t>level_4_intro_0</t>
   </si>
   <si>
@@ -322,21 +253,12 @@
     <t>level_4_switch_instruct_0</t>
   </si>
   <si>
-    <t>Press these two switches to divert the water’s flow towards the bell.</t>
-  </si>
-  <si>
     <t>level_4_goal_thing_0</t>
   </si>
   <si>
-    <t>Excellent! So long as there’s water flowing, the bell will continue to ring.</t>
-  </si>
-  <si>
     <t>level_4_goal_other_pointers_0</t>
   </si>
   <si>
-    <t>Now why don’t you go ahead and let the water flow towards the other bells!</t>
-  </si>
-  <si>
     <t>level_5_intro_0</t>
   </si>
   <si>
@@ -346,12 +268,6 @@
     <t>level_5_intro_2</t>
   </si>
   <si>
-    <t>level_5_intro_3</t>
-  </si>
-  <si>
-    <t>For this one, we will be powering up the bells with electricity.</t>
-  </si>
-  <si>
     <t>Electricity is a kind of energy that can move through conductive materials like metal.</t>
   </si>
   <si>
@@ -391,21 +307,6 @@
     <t>level_5_coal_interact_1</t>
   </si>
   <si>
-    <t>level_5_electric_explain_0</t>
-  </si>
-  <si>
-    <t>level_5_electric_explain_1</t>
-  </si>
-  <si>
-    <t>level_5_electric_explain_2</t>
-  </si>
-  <si>
-    <t>level_5_electric_explain_3</t>
-  </si>
-  <si>
-    <t>Now you’re wondering why go through all this trouble?</t>
-  </si>
-  <si>
     <t>level_5_coal_intro_0</t>
   </si>
   <si>
@@ -427,12 +328,6 @@
     <t>level_5_power_connect_instruct_1</t>
   </si>
   <si>
-    <t>Now let’s power up that bell by attaching the power line into the socket.</t>
-  </si>
-  <si>
-    <t>Simply drag the power plug into the socket as shown.</t>
-  </si>
-  <si>
     <t>level_5_goal_first_active_0</t>
   </si>
   <si>
@@ -442,9 +337,6 @@
     <t>level_5_goal_first_active_2</t>
   </si>
   <si>
-    <t>Excellent! Now we just need to power up the rest of the bells!</t>
-  </si>
-  <si>
     <t>Though you may have noticed that only one of the power lines were able to receive electricity.</t>
   </si>
   <si>
@@ -475,102 +367,24 @@
     <t>level_5_end_1</t>
   </si>
   <si>
-    <t>level_5_end_2</t>
-  </si>
-  <si>
-    <t>Nicely done! With all the bells ringing, we have reached the end of our journey.</t>
-  </si>
-  <si>
     <t>This concludes our lesson for energy movement!</t>
   </si>
   <si>
-    <t>Now go forth, and bring energy into the real world!</t>
-  </si>
-  <si>
-    <t>Here we are near the end of our journey!</t>
-  </si>
-  <si>
     <t>end_thanks</t>
   </si>
   <si>
     <t>Thank you for playing!</t>
   </si>
   <si>
-    <t>This world looks rather gloomy…we ought to brighten things up!</t>
-  </si>
-  <si>
-    <t>Well, for that to happen we need the mighty Aries…who is currently asleep over there.</t>
-  </si>
-  <si>
-    <t>In order to wake him up, we’re going to need to give him some energy!</t>
-  </si>
-  <si>
-    <t>It looks like it’s up to you to take action! With your own energy, help the mighty Aries bring light to this world!</t>
-  </si>
-  <si>
     <t>Energy comes in many forms, and they have ways of moving about.</t>
   </si>
   <si>
-    <t>Light is an energy made up of waves. Among many things, it can provide heat.</t>
-  </si>
-  <si>
-    <t>Think of the sun as the biggest source of light energy, bringing sustenance to most living things.</t>
-  </si>
-  <si>
-    <t>Here we have a spirit that provides light energy.</t>
-  </si>
-  <si>
-    <t>In order for its light energy to move, we’ll need to rotate these contraptions.</t>
-  </si>
-  <si>
-    <t>Excellent! Now that the light energy is free, why don’t we check back with the mighty Aries!</t>
-  </si>
-  <si>
-    <t>Thanks to your efforts, Aries is now full of energy!</t>
-  </si>
-  <si>
-    <t>Now the mighty Aries can go forth to brighten up this world!</t>
-  </si>
-  <si>
-    <t>Let’s help him out further by learning more about energy movements!</t>
-  </si>
-  <si>
-    <t>Now we’ll be learning how to move light energy from one place to another.</t>
-  </si>
-  <si>
-    <t>One neat thing about light is that it can bounce off of reflective surfaces like gems or mirrors.</t>
-  </si>
-  <si>
-    <t>Our task is to redirect the light energy towards this bell.</t>
-  </si>
-  <si>
-    <t>This gem here will bounce the light energy to where it points.</t>
-  </si>
-  <si>
-    <t>Due to the light, the bell is able to vibrate causing it to make another type of energy: sound.</t>
-  </si>
-  <si>
-    <t>But of course, none of this is possible without your actions. Your own energy is what brings these to life!</t>
-  </si>
-  <si>
-    <t>Now to power up the remaining bell!</t>
-  </si>
-  <si>
-    <t>Just like before, place the gems into the slots, and redirect the light energy towards the bell.</t>
-  </si>
-  <si>
     <t>Moving objects contain energy. When it hits another object, that energy is transferred.</t>
   </si>
   <si>
     <t>This is called energy of motion, also known as: kinetic energy.</t>
   </si>
   <si>
-    <t>Nicely done! As you can see, the energy of motion moved from one object to another.</t>
-  </si>
-  <si>
-    <t>Now let’s see if you can ring these other bells!</t>
-  </si>
-  <si>
     <t>Here we have a spirit that provides us an everlasting flow of water.</t>
   </si>
   <si>
@@ -592,46 +406,160 @@
     <t>Well, that’s what these coals are for. Coals provide fire with the energy to release heat.</t>
   </si>
   <si>
-    <t>Well, electrical energy is really easy to move at a long distance. Think of the electrical poles around your home.</t>
-  </si>
-  <si>
-    <t>All that electricity comes from a place far away so it can have enough space to generate lots of energy!</t>
-  </si>
-  <si>
-    <t>Nice! Here you see the whole process of energy moving from one thing to the next, and finally transforming into electricity.</t>
-  </si>
-  <si>
     <t>We need to feed the fire with more oxygen so that it can burn through the coal faster, and produce more heat.</t>
   </si>
   <si>
     <t>With more heat, the water will produce more steam, allowing it to turn the turbine’s fan faster.</t>
   </si>
   <si>
-    <t>Simply press the wind fella multiple times until all the power lines are fully charged with electricity.</t>
-  </si>
-  <si>
     <t>Excellent! With the turbine fully powered, you can now plug in the rest of the power lines.</t>
   </si>
   <si>
-    <t>Just like before, simply drag the power plug into one of the sockets that connects to the bell.</t>
-  </si>
-  <si>
     <t>Also remember to keep the fire well fed with coal and oxygen!</t>
   </si>
   <si>
-    <t>Let me adjust this so that it can hit the second platform!</t>
-  </si>
-  <si>
     <t>You’re going to need to adjust the position of this rock in order to hit both bells.</t>
   </si>
   <si>
     <t>The energy released from the spring plunger has caused a series of movement, from one rock to another.</t>
   </si>
   <si>
-    <t>As you can see, we are able to change from one energy into another. It changes from light to sound energy.</t>
-  </si>
-  <si>
-    <t>Phew! That’s a lot of energy movement from one thing to another!</t>
+    <t>test_0</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Press and hold the highlighted lever, and move it towards the top.</t>
+  </si>
+  <si>
+    <t>level_1_outer_0</t>
+  </si>
+  <si>
+    <t>level_1_inner_complete_1</t>
+  </si>
+  <si>
+    <t>level_1_inner_complete_2</t>
+  </si>
+  <si>
+    <t>As you can see, light can pass through the glass.</t>
+  </si>
+  <si>
+    <t>Now we just need to turn the other contraption to allow the light to shine through!</t>
+  </si>
+  <si>
+    <t>Excellent! Now that the light energy is shining through, why don’t we check back down below.</t>
+  </si>
+  <si>
+    <t>Welcome! I’ve brought you to this world in order to set things right.</t>
+  </si>
+  <si>
+    <t>As you can see, this place is rather gloomy.</t>
+  </si>
+  <si>
+    <t>We need your help to bring energy to this world by waking up this sheep here called Aries.</t>
+  </si>
+  <si>
+    <t>Now let us take to the skies, and activate the artifact to wake Aries up!</t>
+  </si>
+  <si>
+    <t>Which makes sense, since our eyes can see things when there is light.</t>
+  </si>
+  <si>
+    <t>A glass is a kind of material that is highly transparent. Meaning you can see through it with ease.</t>
+  </si>
+  <si>
+    <t>Filled with energy from the light, Aries is now ready to go!</t>
+  </si>
+  <si>
+    <t>Let’s help him out further by activating the other artifacts in the sky.</t>
+  </si>
+  <si>
+    <t>Light is an energy made up of waves. It can travel through space and air.</t>
+  </si>
+  <si>
+    <t>However, it is currently being blocked. Let’s fix that by turning these round contraptions.</t>
+  </si>
+  <si>
+    <t>Now let’s take a look at how to move light energy from one place to another.</t>
+  </si>
+  <si>
+    <t>One thing about light is that it can bounce off of reflective surfaces like mirrors.</t>
+  </si>
+  <si>
+    <t>Our task is to redirect the light energy towards this speaker.</t>
+  </si>
+  <si>
+    <t>This gadget has a reflective surface that will bounce the light towards where we want it to go.</t>
+  </si>
+  <si>
+    <t>Press and drag the gadget towards the available slot.</t>
+  </si>
+  <si>
+    <t>Excellent! As you can see, the light is bouncing off of the reflective surface of the gadget.</t>
+  </si>
+  <si>
+    <t>Go ahead, and place the next gadget like the previous one.</t>
+  </si>
+  <si>
+    <t>This time around, you’ll need to redirect the reflection towards the speaker.</t>
+  </si>
+  <si>
+    <t>level_2_gem_next_placed_1</t>
+  </si>
+  <si>
+    <t>To do that, you must press and drag the lever as shown.</t>
+  </si>
+  <si>
+    <t>Nice! As you can see and hear, the speaker is playing a tune.</t>
+  </si>
+  <si>
+    <t>Energy can be changed from one form into another.</t>
+  </si>
+  <si>
+    <t>In this case, the speaker is using light energy to power itself up to produce sound energy.</t>
+  </si>
+  <si>
+    <t>Now to power up the other speaker. Just like before, we need to redirect the light towards the speaker.</t>
+  </si>
+  <si>
+    <t>Now let’s see if you can power up these speakers.</t>
+  </si>
+  <si>
+    <t>As you can see, the energy of motion moved from one object to another.</t>
+  </si>
+  <si>
+    <t>Press these two switches to divert the water’s flow to power up the speaker.</t>
+  </si>
+  <si>
+    <t>Go ahead and power up the other speakers by diverting more of the water’s flow!</t>
+  </si>
+  <si>
+    <t>Here we are with our last sky artifact. We will be powering up the speakers with electricity!</t>
+  </si>
+  <si>
+    <t>Here you see the whole process of energy changing from one thing to another, and finally into electricity.</t>
+  </si>
+  <si>
+    <t>Now let’s power up that speaker by attaching the power line into the socket.</t>
+  </si>
+  <si>
+    <t>Press and drag the power plug into the socket as shown.</t>
+  </si>
+  <si>
+    <t>Excellent! Now we just need to power up the rest of the speakers!</t>
+  </si>
+  <si>
+    <t>Press the wind spirit multiple times until all the power lines are fully charged with electricity.</t>
+  </si>
+  <si>
+    <t>Just like before, press and drag the power plug into one of the sockets that connects to the bell.</t>
+  </si>
+  <si>
+    <t>Nicely done! With all the speakers powered up, we have activated the last artifact.</t>
+  </si>
+  <si>
+    <t>As you can see, the water’s continuous flow is powering up the speaker.</t>
   </si>
 </sst>
 </file>
@@ -970,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,10 +1024,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1107,7 +1035,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1115,55 +1043,55 @@
         <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>160</v>
+      <c r="B17" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>161</v>
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>162</v>
+        <v>35</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>163</v>
+        <v>37</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1171,500 +1099,500 @@
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>166</v>
+        <v>139</v>
+      </c>
+      <c r="B25" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
+        <v>137</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" t="s">
-        <v>168</v>
+        <v>42</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" t="s">
-        <v>169</v>
+        <v>43</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" t="s">
-        <v>170</v>
+        <v>50</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" t="s">
-        <v>171</v>
+        <v>44</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" t="s">
-        <v>172</v>
+        <v>45</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" t="s">
-        <v>173</v>
+        <v>46</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" t="s">
-        <v>174</v>
+        <v>47</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>59</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>63</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" t="s">
-        <v>65</v>
+        <v>52</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>67</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>94</v>
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>175</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>202</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
-      </c>
-      <c r="B47" t="s">
-        <v>177</v>
+        <v>58</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" t="s">
-        <v>178</v>
+        <v>59</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" t="s">
-        <v>92</v>
+        <v>62</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>180</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>78</v>
-      </c>
-      <c r="B52" t="s">
-        <v>93</v>
+        <v>66</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B56" t="s">
-        <v>181</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
-        <v>201</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" t="s">
-        <v>182</v>
+        <v>76</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>200</v>
+        <v>78</v>
+      </c>
+      <c r="B60" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>97</v>
-      </c>
-      <c r="B63" t="s">
-        <v>183</v>
+        <v>81</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>98</v>
-      </c>
-      <c r="B64" t="s">
-        <v>184</v>
+        <v>84</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>99</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>100</v>
+        <v>85</v>
+      </c>
+      <c r="B65" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>101</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>102</v>
+        <v>87</v>
+      </c>
+      <c r="B66" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>105</v>
-      </c>
-      <c r="B68" t="s">
-        <v>155</v>
+        <v>90</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>107</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>110</v>
+        <v>95</v>
+      </c>
+      <c r="B70" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>108</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>111</v>
+        <v>96</v>
+      </c>
+      <c r="B71" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>113</v>
-      </c>
-      <c r="B73" t="s">
-        <v>185</v>
+        <v>94</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>115</v>
-      </c>
-      <c r="B74" t="s">
-        <v>186</v>
+        <v>99</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>120</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>128</v>
-      </c>
-      <c r="B78" t="s">
-        <v>188</v>
+        <v>103</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>129</v>
-      </c>
-      <c r="B79" t="s">
-        <v>189</v>
+        <v>104</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B80" t="s">
-        <v>203</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>125</v>
-      </c>
-      <c r="B82" t="s">
-        <v>190</v>
+        <v>109</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>126</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>191</v>
+        <v>110</v>
+      </c>
+      <c r="B83" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>131</v>
@@ -1672,130 +1600,34 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>132</v>
-      </c>
-      <c r="B86" t="s">
-        <v>192</v>
+        <v>113</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>138</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>139</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>143</v>
-      </c>
-      <c r="B92" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>144</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>145</v>
-      </c>
-      <c r="B94" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>146</v>
-      </c>
-      <c r="B95" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>147</v>
-      </c>
-      <c r="B96" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>148</v>
-      </c>
-      <c r="B97" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>149</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>150</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>151</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>156</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>